<commit_message>
pushed code with log 23/9/22
</commit_message>
<xml_diff>
--- a/Config/MarketoData.xlsx
+++ b/Config/MarketoData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="48">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Nurture campaigns</t>
   </si>
   <si>
-    <t>Library</t>
-  </si>
-  <si>
     <t>Web Personalize</t>
   </si>
   <si>
@@ -161,6 +158,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Programe Library</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -540,7 +543,7 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
@@ -554,12 +557,12 @@
         <v>2.0</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="n">
         <v>2.0</v>
@@ -568,12 +571,12 @@
         <v>2.0</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="n">
         <v>3.0</v>
@@ -582,12 +585,12 @@
         <v>3.0</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -596,12 +599,12 @@
         <v>1.0</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="n">
         <v>0.0</v>
@@ -610,129 +613,171 @@
         <v>0.0</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
       <c r="B9" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
       <c r="B10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
       <c r="B11" t="n">
         <v>0.0</v>
       </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
       <c r="B12" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
       <c r="B13" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
       <c r="B14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" t="n">
-        <v>0.0</v>
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2.0</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" t="n">
-        <v>0.0</v>
+      <c r="A17" t="s">
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
       <c r="B19" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E19" t="n">
         <v>0.0</v>
       </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
@@ -788,36 +833,36 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
-        <v>2</v>
+      <c r="B28" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
-        <v>3</v>
+      <c r="B29" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -825,7 +870,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -833,7 +878,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Support Tools changes and Design studio Count window changes
</commit_message>
<xml_diff>
--- a/Config/MarketoData.xlsx
+++ b/Config/MarketoData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032691E5-D3B5-4434-9B58-50555D7179EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="3600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7766" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="72">
   <si>
     <t>Interesting Moment</t>
   </si>
@@ -42,6 +43,12 @@
     <t>1</t>
   </si>
   <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>Landing Pages</t>
+  </si>
+  <si>
     <t>All Campaigns</t>
   </si>
   <si>
@@ -51,6 +58,9 @@
     <t>Active Triggered Campaigns</t>
   </si>
   <si>
+    <t>Tags</t>
+  </si>
+  <si>
     <t>All Triggered Campaigns</t>
   </si>
   <si>
@@ -63,9 +73,21 @@
     <t>All Batch Campaigns</t>
   </si>
   <si>
+    <t>Images and Files</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
+    <t>Snippets</t>
+  </si>
+  <si>
+    <t>Segmentations</t>
+  </si>
+  <si>
     <t>Integration</t>
   </si>
   <si>
@@ -87,6 +109,9 @@
     <t>9</t>
   </si>
   <si>
+    <t>Models</t>
+  </si>
+  <si>
     <t>Default</t>
   </si>
   <si>
@@ -102,76 +127,121 @@
     <t>WP_DEMO</t>
   </si>
   <si>
+    <t>Asset Data</t>
+  </si>
+  <si>
+    <t>Database Data</t>
+  </si>
+  <si>
+    <t>Program Data</t>
+  </si>
+  <si>
+    <t>Total WorkSpace</t>
+  </si>
+  <si>
     <t>Event Programs</t>
   </si>
   <si>
     <t>Nurture campaigns</t>
   </si>
   <si>
-    <t>Library</t>
-  </si>
-  <si>
-    <t>Web Personalize</t>
-  </si>
-  <si>
-    <t>Target Account Management</t>
-  </si>
-  <si>
-    <t>Predictive Content</t>
-  </si>
-  <si>
-    <t>Forms</t>
-  </si>
-  <si>
-    <t>Landing Pages</t>
-  </si>
-  <si>
-    <t>Images and Files</t>
-  </si>
-  <si>
-    <t>Snippets</t>
-  </si>
-  <si>
-    <t>Asset Data</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>Segmentations</t>
-  </si>
-  <si>
-    <t>Leads</t>
-  </si>
-  <si>
-    <t>Database Data</t>
-  </si>
-  <si>
-    <t>Models</t>
-  </si>
-  <si>
-    <t>Program Data</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>Total WorkSpace</t>
+    <t>180</t>
+  </si>
+  <si>
+    <t>.Customer Support New Hire Workspace</t>
+  </si>
+  <si>
+    <t>ACT-SS</t>
+  </si>
+  <si>
+    <t>Alicia's Ally</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Alicia's Default</t>
+  </si>
+  <si>
+    <t>Amenefees Workspace</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>C.COEL</t>
+  </si>
+  <si>
+    <t>Calvin_Support_Workspace</t>
+  </si>
+  <si>
+    <t>Chris Davis</t>
+  </si>
+  <si>
+    <t>Chris_WorkSpace</t>
+  </si>
+  <si>
+    <t>cpanella</t>
+  </si>
+  <si>
+    <t>Customer Partition</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>Cyndie's Work Space</t>
+  </si>
+  <si>
+    <t>Ed's Workplace</t>
+  </si>
+  <si>
+    <t>EMEA CSM</t>
+  </si>
+  <si>
+    <t>French workspace</t>
+  </si>
+  <si>
+    <t>Gabrielle M's Workspace</t>
+  </si>
+  <si>
+    <t>Japan CSM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2690</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>Pradyumna Sahoo</t>
   </si>
   <si>
     <t>Programe Library</t>
   </si>
   <si>
-    <t>False</t>
+    <t>37</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -514,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A31" sqref="A31:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,346 +605,352 @@
       </c>
     </row>
     <row r="2">
-      <c r="E2" t="s">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="n">
+        <v>165.0</v>
+      </c>
       <c r="C3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
+        <v>7.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>56.0</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
       </c>
-      <c r="E4" t="s">
-        <v>45</v>
+      <c r="D4" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>71.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
+        <v>7.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="n">
+        <v>582.0</v>
       </c>
       <c r="C6" t="n">
         <v>1.0</v>
       </c>
-      <c r="E6" t="s">
-        <v>45</v>
+      <c r="D6" t="n">
+        <v>581.0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7">
-      <c r="E7" t="s">
-        <v>45</v>
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="U7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" t="n">
         <v>0.0</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
       <c r="B13" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C13" t="s">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+      <c r="D18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
       <c r="E18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19" t="n">
         <v>1.0</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.0</v>
+      <c r="E19">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
-      <c r="B25" t="n">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="26">
+      <c r="B25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" t="n">
-        <v>1.0</v>
+      <c r="B26">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B29" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>243.0</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" t="b">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final merge on 11/9/2022
</commit_message>
<xml_diff>
--- a/Config/MarketoData.xlsx
+++ b/Config/MarketoData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22620" windowHeight="5760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22620" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="47">
   <si>
     <t>VALUE</t>
   </si>
@@ -61,36 +61,18 @@
     <t>Event Programs</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>ACT-SS</t>
-  </si>
-  <si>
-    <t>.Customer Support New Hire Workspace</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
     <t>Programe Library</t>
   </si>
   <si>
-    <t>Pradyumna Sahoo</t>
-  </si>
-  <si>
     <t>Models</t>
   </si>
   <si>
     <t>All Triggered Campaigns</t>
   </si>
   <si>
-    <t>37</t>
-  </si>
-  <si>
     <t>Active Triggered Campaigns</t>
   </si>
   <si>
@@ -103,39 +85,21 @@
     <t>All Batch Campaigns</t>
   </si>
   <si>
-    <t>82</t>
-  </si>
-  <si>
     <t>All Campaigns</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>Active Campaigns</t>
   </si>
   <si>
     <t>Campaign Data</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Nurture campaigns</t>
   </si>
   <si>
-    <t>2706</t>
-  </si>
-  <si>
     <t>Total WorkSpace</t>
   </si>
   <si>
-    <t>2710</t>
-  </si>
-  <si>
     <t>Emails</t>
   </si>
   <si>
@@ -172,31 +136,31 @@
     <t>6</t>
   </si>
   <si>
+    <t>sandboxcopy clone07</t>
+  </si>
+  <si>
+    <t>WP_DEMO</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Change Score</t>
+  </si>
+  <si>
+    <t>Interesting Moment</t>
+  </si>
+  <si>
+    <t>Change Data Value</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>sandboxcopy clone07</t>
-  </si>
-  <si>
-    <t>WP_DEMO</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Change Score</t>
+    <t>Test</t>
   </si>
   <si>
     <t>58</t>
-  </si>
-  <si>
-    <t>Interesting Moment</t>
-  </si>
-  <si>
-    <t>Change Data Value</t>
-  </si>
-  <si>
-    <t>1354</t>
   </si>
 </sst>
 </file>
@@ -546,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,226 +531,244 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B3" t="n">
-        <v>165.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>158.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>56.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" t="n">
-        <v>54.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>75.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" t="n">
-        <v>68.0</v>
+        <v>3.0</v>
       </c>
       <c r="D5" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>582.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" t="n">
-        <v>581.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>40.0</v>
+        <v>65.0</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B11" t="n">
         <v>0.0</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>84.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>128.0</v>
+        <v>67.0</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -794,47 +776,56 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C16" t="n">
         <v>2.0</v>
       </c>
       <c r="D16" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="n">
-        <v>262.0</v>
+        <v>964.0</v>
       </c>
       <c r="C17" t="n">
-        <v>131.0</v>
+        <v>241.0</v>
       </c>
       <c r="D17" t="n">
-        <v>131.0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
+        <v>241.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>241.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>241.0</v>
       </c>
     </row>
     <row r="18">
@@ -845,30 +836,36 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B19" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C19" t="n">
         <v>1.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
+        <v>1.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -884,7 +881,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22">
@@ -900,30 +897,39 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="28">
@@ -931,23 +937,23 @@
         <v>12</v>
       </c>
       <c r="B28" t="n">
-        <v>250.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B29" t="n">
-        <v>248.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new code for full screen screenshot, PC screenshot
</commit_message>
<xml_diff>
--- a/Config/MarketoData.xlsx
+++ b/Config/MarketoData.xlsx
@@ -19,7 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9570" uniqueCount="74">
+  <si>
+    <t>Interesting Moment</t>
+  </si>
+  <si>
+    <t>Change Data Value</t>
+  </si>
   <si>
     <t>VALUE</t>
   </si>
@@ -27,160 +33,214 @@
     <t>KEY COMPNENT</t>
   </si>
   <si>
+    <t>Change Score</t>
+  </si>
+  <si>
+    <t>Emails</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>All Campaigns</t>
+  </si>
+  <si>
+    <t>Active Campaigns</t>
+  </si>
+  <si>
+    <t>Active Triggered Campaigns</t>
+  </si>
+  <si>
+    <t>All Triggered Campaigns</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Batch Campaigns - Repeating Schedule</t>
+  </si>
+  <si>
+    <t>All Batch Campaigns</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Interesting Moment Subscription</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>sandboxcopy_23may_07 Marketo</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>Default</t>
   </si>
   <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Campaign Data</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
+    <t>WP_DEMO</t>
+  </si>
+  <si>
+    <t>Event Programs</t>
+  </si>
+  <si>
+    <t>Nurture campaigns</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Web Personalize</t>
+  </si>
+  <si>
+    <t>Target Account Management</t>
+  </si>
+  <si>
+    <t>Predictive Content</t>
+  </si>
+  <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>Landing Pages</t>
+  </si>
+  <si>
+    <t>Images and Files</t>
+  </si>
+  <si>
+    <t>Snippets</t>
+  </si>
+  <si>
     <t>Asset Data</t>
   </si>
   <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Segmentations</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>Database Data</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Program Data</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>Total WorkSpace</t>
+  </si>
+  <si>
+    <t>Programe Library</t>
+  </si>
+  <si>
     <t>False</t>
   </si>
   <si>
+    <t>369</t>
+  </si>
+  <si>
+    <t>19augsub001 Marketo</t>
+  </si>
+  <si>
+    <t>WS A</t>
+  </si>
+  <si>
+    <t>SanjayTest</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>sandboxcopy clone07</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>2267</t>
+  </si>
+  <si>
+    <t>915</t>
+  </si>
+  <si>
     <t>138</t>
   </si>
   <si>
     <t>473</t>
   </si>
   <si>
+    <t>2806</t>
+  </si>
+  <si>
+    <t>1078</t>
+  </si>
+  <si>
+    <t>1153</t>
+  </si>
+  <si>
     <t>14</t>
   </si>
   <si>
+    <t>Deputec Pty Limited Marketo</t>
+  </si>
+  <si>
+    <t>Approved Models1</t>
+  </si>
+  <si>
+    <t>Acquisition with Upsell Lifecycle-NEW</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
+    <t>133</t>
+  </si>
+  <si>
     <t>429</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>2269</t>
-  </si>
-  <si>
-    <t>917</t>
-  </si>
-  <si>
-    <t>2808</t>
-  </si>
-  <si>
-    <t>1080</t>
-  </si>
-  <si>
-    <t>1154</t>
-  </si>
-  <si>
-    <t>Deputec Pty Limited Marketo</t>
-  </si>
-  <si>
-    <t>Acquisition with Upsell Lifecycle-NEW</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>6478</t>
-  </si>
-  <si>
-    <t>tesr</t>
-  </si>
-  <si>
-    <t>All Triggered Campaigns</t>
-  </si>
-  <si>
-    <t>Active Triggered Campaigns</t>
-  </si>
-  <si>
-    <t>Batch Campaigns - Repeating Schedule</t>
-  </si>
-  <si>
-    <t>All Batch Campaigns</t>
-  </si>
-  <si>
-    <t>All Campaigns</t>
-  </si>
-  <si>
-    <t>Active Campaigns</t>
-  </si>
-  <si>
-    <t>Campaign Data</t>
-  </si>
-  <si>
-    <t>Total WorkSpace</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Integration</t>
-  </si>
-  <si>
-    <t>Interesting Moment Subscription</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Models</t>
-  </si>
-  <si>
-    <t>Approved Models1</t>
-  </si>
-  <si>
-    <t>Program Data</t>
-  </si>
-  <si>
-    <t>Segmentations</t>
-  </si>
-  <si>
-    <t>Leads</t>
-  </si>
-  <si>
-    <t>Database Data</t>
-  </si>
-  <si>
-    <t>Emails</t>
-  </si>
-  <si>
-    <t>Forms</t>
-  </si>
-  <si>
-    <t>Landing Pages</t>
-  </si>
-  <si>
-    <t>Images and Files</t>
-  </si>
-  <si>
-    <t>Snippets</t>
-  </si>
-  <si>
-    <t>Event Programs</t>
-  </si>
-  <si>
-    <t>Nurture campaigns</t>
-  </si>
-  <si>
-    <t>Programe Library</t>
-  </si>
-  <si>
-    <t>Target Account Management</t>
-  </si>
-  <si>
-    <t>Predictive Content</t>
-  </si>
-  <si>
-    <t>Change Score</t>
-  </si>
-  <si>
-    <t>Interesting Moment</t>
-  </si>
-  <si>
-    <t>Change Data Value</t>
+    <t>6477</t>
   </si>
 </sst>
 </file>
@@ -530,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,43 +603,43 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1581.0</v>
+        <v>1580.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1581.0</v>
+        <v>1580.0</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" t="n">
         <v>381.0</v>
@@ -588,12 +648,12 @@
         <v>381.0</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B5" t="n">
         <v>225.0</v>
@@ -602,12 +662,12 @@
         <v>225.0</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B6" t="n">
         <v>2101.0</v>
@@ -616,138 +676,138 @@
         <v>2101.0</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B7" t="n">
         <v>15.0</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>2269.0</v>
+        <v>2267.0</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>917.0</v>
+        <v>915.0</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
         <v>138.0</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B12" t="n">
         <v>473.0</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>2808.0</v>
+        <v>2806.0</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>1080.0</v>
+        <v>1078.0</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" t="n">
         <v>8.0</v>
@@ -756,163 +816,172 @@
         <v>8.0</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" t="n">
-        <v>1065771.0</v>
+        <v>1063254.0</v>
       </c>
       <c r="C17" t="n">
-        <v>1065771.0</v>
+        <v>1063254.0</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B19" t="n">
         <v>2.0</v>
       </c>
-      <c r="C19" t="n">
-        <v>2.0</v>
-      </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B27" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" t="s">
-        <v>5</v>
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>76.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" t="s">
-        <v>5</v>
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>38.0</v>
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C35" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>19</v>
+      <c r="D35" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>